<commit_message>
Add ND_Acq saturation limits
</commit_message>
<xml_diff>
--- a/notebooks/SatLimits_Coronagraph.xlsx
+++ b/notebooks/SatLimits_Coronagraph.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwstnircam/Dropbox/NIRCam/pynrc/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwstnircam/GitHub/pynrc/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19360" yWindow="6060" windowWidth="20020" windowHeight="17140" tabRatio="500"/>
+    <workbookView xWindow="21880" yWindow="3960" windowWidth="28080" windowHeight="17140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CIRCLYOT" sheetId="1" r:id="rId1"/>
+    <sheet name="NDSQUARE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="39">
   <si>
     <t>MASK210R (640x640)</t>
   </si>
@@ -119,10 +120,31 @@
     <t>MASK335R (320x320)</t>
   </si>
   <si>
-    <t>SW Coronagraphy Saturation Limits (CIRCLYOT)</t>
-  </si>
-  <si>
-    <t>LW Coronagraphy Saturation Limits (CIRCLYOT)</t>
+    <t>SW Coronagraphy K-Band Saturation Limits (CIRCLYOT)</t>
+  </si>
+  <si>
+    <t>LW Coronagraphy K-Band Saturation Limits (CIRCLYOT)</t>
+  </si>
+  <si>
+    <t>SW Coronagraphy K-Band Saturation Limits (ND Acqusition)</t>
+  </si>
+  <si>
+    <t>LW Coronagraphy K-Band Saturation Limits (ND Acquisition)</t>
+  </si>
+  <si>
+    <t>NDSQUARE (640x640)</t>
+  </si>
+  <si>
+    <t>NDSQUARE (320x320)</t>
+  </si>
+  <si>
+    <t>ND Acquisition K-Band Saturation Limits</t>
+  </si>
+  <si>
+    <t>SW Filters (128x128)</t>
+  </si>
+  <si>
+    <t>LW Filters (64x64)</t>
   </si>
 </sst>
 </file>
@@ -269,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -284,12 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -305,6 +321,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,75 +606,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="K3" s="12" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="F4" s="13" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="F4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="K4" s="13" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+      <c r="K4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="16"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -660,7 +689,7 @@
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="2" t="s">
         <v>3</v>
       </c>
@@ -670,7 +699,7 @@
       <c r="I5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="14"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="2" t="s">
         <v>3</v>
       </c>
@@ -686,37 +715,37 @@
         <v>6</v>
       </c>
       <c r="B6" s="5">
-        <v>1.97840494129</v>
+        <v>1.73</v>
       </c>
       <c r="C6" s="5">
-        <v>2.4704485963699998</v>
+        <v>2.29</v>
       </c>
       <c r="D6" s="6">
-        <v>2.6668147487599998</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="5">
-        <v>0.62956107417100005</v>
+        <v>0.45</v>
       </c>
       <c r="H6" s="5">
-        <v>1.1195539746100001</v>
+        <v>0.94</v>
       </c>
       <c r="I6" s="6">
-        <v>1.3144695990699999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L6" s="5">
-        <v>-0.85241059683099996</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="M6" s="5">
-        <v>-0.362417696397</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="N6" s="6">
-        <v>-0.16750207193300001</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -724,37 +753,37 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>2.9829962445299998</v>
+        <v>2.67</v>
       </c>
       <c r="C7" s="5">
-        <v>2.9343776043899998</v>
+        <v>2.69</v>
       </c>
       <c r="D7" s="6">
-        <v>2.9508321718500001</v>
+        <v>2.7</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="5">
-        <v>1.9188657418699999</v>
+        <v>1.68</v>
       </c>
       <c r="H7" s="5">
-        <v>1.86858909584</v>
+        <v>1.63</v>
       </c>
       <c r="I7" s="6">
-        <v>1.88427842503</v>
+        <v>1.64</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L7" s="5">
-        <v>0.43689407086400001</v>
+        <v>0.13</v>
       </c>
       <c r="M7" s="5">
-        <v>0.38661742483400002</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="N7" s="6">
-        <v>0.40230675402900001</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -762,37 +791,37 @@
         <v>8</v>
       </c>
       <c r="B8" s="5">
-        <v>2.6322526801700001</v>
+        <v>2.35</v>
       </c>
       <c r="C8" s="5">
-        <v>2.56839127224</v>
+        <v>2.35</v>
       </c>
       <c r="D8" s="6">
-        <v>2.5750287678400001</v>
+        <v>2.36</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="5">
-        <v>1.65665975297</v>
+        <v>1.43</v>
       </c>
       <c r="H8" s="5">
-        <v>1.5926672288199999</v>
+        <v>1.37</v>
       </c>
       <c r="I8" s="6">
-        <v>1.5962724659400001</v>
+        <v>1.38</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L8" s="5">
-        <v>0.174688081971</v>
+        <v>-0.12</v>
       </c>
       <c r="M8" s="5">
-        <v>0.110695557816</v>
+        <v>-0.12</v>
       </c>
       <c r="N8" s="6">
-        <v>0.11430079493799999</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -800,37 +829,37 @@
         <v>9</v>
       </c>
       <c r="B9" s="5">
-        <v>0.155779232988</v>
+        <v>0.03</v>
       </c>
       <c r="C9" s="5">
-        <v>2.6492364190100002</v>
+        <v>2.59</v>
       </c>
       <c r="D9" s="6">
-        <v>3.6488733310899999</v>
+        <v>3.59</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="5">
-        <v>-1.4971002958999999</v>
+        <v>-1.55</v>
       </c>
       <c r="H9" s="5">
-        <v>0.83728282553300004</v>
+        <v>0.78</v>
       </c>
       <c r="I9" s="6">
-        <v>1.8356665883300001</v>
+        <v>1.78</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="5">
-        <v>-2.9790719668999999</v>
+        <v>-3.1</v>
       </c>
       <c r="M9" s="5">
-        <v>-0.64468884546899996</v>
+        <v>-0.7</v>
       </c>
       <c r="N9" s="6">
-        <v>0.35369491732899999</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -838,37 +867,37 @@
         <v>10</v>
       </c>
       <c r="B10" s="5">
-        <v>2.0773662496599998</v>
+        <v>1.95</v>
       </c>
       <c r="C10" s="5">
-        <v>3.40786239486</v>
+        <v>3.35</v>
       </c>
       <c r="D10" s="6">
-        <v>4.0548129359000002</v>
+        <v>3.99</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="5">
-        <v>0.445685531405</v>
+        <v>0.39</v>
       </c>
       <c r="H10" s="5">
-        <v>1.80802303247</v>
+        <v>1.75</v>
       </c>
       <c r="I10" s="6">
-        <v>2.4574263407800001</v>
+        <v>2.4</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L10" s="5">
-        <v>-1.0362861396</v>
+        <v>-1.1599999999999999</v>
       </c>
       <c r="M10" s="5">
-        <v>0.32605136146500002</v>
+        <v>0.27</v>
       </c>
       <c r="N10" s="6">
-        <v>0.97545466977899997</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -876,37 +905,37 @@
         <v>11</v>
       </c>
       <c r="B11" s="5">
-        <v>2.80178020459</v>
+        <v>2.66</v>
       </c>
       <c r="C11" s="5">
-        <v>3.7388502217299999</v>
+        <v>3.66</v>
       </c>
       <c r="D11" s="6">
-        <v>4.2151670123700002</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="5">
-        <v>1.2745676303</v>
+        <v>1.2</v>
       </c>
       <c r="H11" s="5">
-        <v>2.2081310187500001</v>
+        <v>2.13</v>
       </c>
       <c r="I11" s="6">
-        <v>2.6825209059800001</v>
+        <v>2.61</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="5">
-        <v>-0.207404040698</v>
+        <v>-0.35</v>
       </c>
       <c r="M11" s="5">
-        <v>0.72615934774900004</v>
+        <v>0.65</v>
       </c>
       <c r="N11" s="6">
-        <v>1.20054923497</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -914,37 +943,37 @@
         <v>12</v>
       </c>
       <c r="B12" s="5">
-        <v>3.2538867925899999</v>
+        <v>2.96</v>
       </c>
       <c r="C12" s="5">
-        <v>3.5632074436900001</v>
+        <v>3.34</v>
       </c>
       <c r="D12" s="6">
-        <v>3.6543655232900001</v>
+        <v>3.43</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="5">
-        <v>1.96330626612</v>
+        <v>1.74</v>
       </c>
       <c r="H12" s="5">
-        <v>2.2670441989199999</v>
+        <v>2.04</v>
       </c>
       <c r="I12" s="6">
-        <v>2.3549377688200002</v>
+        <v>2.13</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="5">
-        <v>0.48133459511999999</v>
+        <v>0.19</v>
       </c>
       <c r="M12" s="5">
-        <v>0.78507252791799997</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="N12" s="6">
-        <v>0.87296609781699996</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -952,37 +981,37 @@
         <v>13</v>
       </c>
       <c r="B13" s="5">
-        <v>3.9309023507899998</v>
+        <v>3.64</v>
       </c>
       <c r="C13" s="5">
-        <v>4.2332332148800003</v>
+        <v>4.08</v>
       </c>
       <c r="D13" s="6">
-        <v>4.4991201575800002</v>
+        <v>4.37</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="5">
-        <v>2.7516286897</v>
+        <v>2.52</v>
       </c>
       <c r="H13" s="5">
-        <v>2.95550264298</v>
+        <v>2.79</v>
       </c>
       <c r="I13" s="6">
-        <v>3.1901789120399999</v>
+        <v>3.04</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L13" s="5">
-        <v>1.26965701869</v>
+        <v>0.97</v>
       </c>
       <c r="M13" s="5">
-        <v>1.47353097198</v>
+        <v>1.31</v>
       </c>
       <c r="N13" s="6">
-        <v>1.70820724104</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -990,37 +1019,37 @@
         <v>14</v>
       </c>
       <c r="B14" s="8">
-        <v>3.5062645449300001</v>
+        <v>3.23</v>
       </c>
       <c r="C14" s="8">
-        <v>3.44848860414</v>
+        <v>3.23</v>
       </c>
       <c r="D14" s="9">
-        <v>3.45750588194</v>
+        <v>3.24</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="8">
-        <v>2.3844981502000002</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="H14" s="8">
-        <v>2.3265099903899999</v>
+        <v>2.12</v>
       </c>
       <c r="I14" s="9">
-        <v>2.3362742762900002</v>
+        <v>2.13</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="L14" s="8">
-        <v>0.90252647919700002</v>
+        <v>0.63</v>
       </c>
       <c r="M14" s="8">
-        <v>0.84453831938500001</v>
+        <v>0.64</v>
       </c>
       <c r="N14" s="9">
-        <v>0.85430260528500002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1031,53 +1060,92 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:19" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="K17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+    </row>
+    <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="F19" s="12" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="F19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="K19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="P19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="F20" s="13" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="F20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="16"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="K20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="14"/>
+      <c r="P20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="R20" s="13"/>
+      <c r="S20" s="14"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1155,7 @@
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1097,338 +1165,1348 @@
       <c r="I21" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="12"/>
+      <c r="L21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="5">
-        <v>-0.32345473638599997</v>
+        <v>-0.4</v>
       </c>
       <c r="C22" s="5">
-        <v>-4.9767755027400003E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D22" s="6">
-        <v>-6.5044807990600001E-2</v>
+        <v>-0.08</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="5">
-        <v>0.300755022127</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H22" s="5">
-        <v>0.57482200819499996</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="I22" s="6">
-        <v>0.559670836753</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="5">
+        <v>-3.13</v>
+      </c>
+      <c r="M22" s="5">
+        <v>-2.58</v>
+      </c>
+      <c r="N22" s="6">
+        <v>-2.38</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>-2.48</v>
+      </c>
+      <c r="R22" s="5">
+        <v>-2.14</v>
+      </c>
+      <c r="S22" s="6">
+        <v>-2.16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="5">
-        <v>-0.23632326562799999</v>
+        <v>-0.32</v>
       </c>
       <c r="C23" s="5">
-        <v>-0.33534642268499998</v>
+        <v>-0.35</v>
       </c>
       <c r="D23" s="6">
-        <v>-0.37422822092000002</v>
+        <v>-0.39</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="5">
-        <v>0.32221190949099998</v>
+        <v>0.31</v>
       </c>
       <c r="H23" s="5">
-        <v>0.22127218717200001</v>
+        <v>0.21</v>
       </c>
       <c r="I23" s="6">
-        <v>0.182394870647</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.17</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="5">
+        <v>-1.59</v>
+      </c>
+      <c r="M23" s="5">
+        <v>-1.58</v>
+      </c>
+      <c r="N23" s="6">
+        <v>-1.56</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>-2.2200000000000002</v>
+      </c>
+      <c r="R23" s="5">
+        <v>-2.2599999999999998</v>
+      </c>
+      <c r="S23" s="6">
+        <v>-2.29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="5">
-        <v>-0.41178158881100002</v>
+        <v>-0.49</v>
       </c>
       <c r="C24" s="5">
-        <v>-0.57555638906899997</v>
+        <v>-0.59</v>
       </c>
       <c r="D24" s="6">
-        <v>-0.61999820225400004</v>
+        <v>-0.63</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="5">
-        <v>8.8541469015299995E-2</v>
+        <v>0.08</v>
       </c>
       <c r="H24" s="5">
-        <v>-7.4343059221200006E-2</v>
+        <v>-0.08</v>
       </c>
       <c r="I24" s="6">
-        <v>-0.118749370659</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-0.13</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="5">
+        <v>-1.67</v>
+      </c>
+      <c r="M24" s="5">
+        <v>-1.67</v>
+      </c>
+      <c r="N24" s="6">
+        <v>-1.66</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>-2.25</v>
+      </c>
+      <c r="R24" s="5">
+        <v>-2.35</v>
+      </c>
+      <c r="S24" s="6">
+        <v>-2.39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="5">
-        <v>-0.54428214995500002</v>
+        <v>-0.62</v>
       </c>
       <c r="C25" s="5">
-        <v>-0.716120383157</v>
+        <v>-0.73</v>
       </c>
       <c r="D25" s="6">
-        <v>-0.76810582873099997</v>
+        <v>-0.78</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G25" s="5">
-        <v>-9.2432057077299998E-2</v>
+        <v>-0.1</v>
       </c>
       <c r="H25" s="5">
-        <v>-0.26422263984099997</v>
+        <v>-0.27</v>
       </c>
       <c r="I25" s="6">
-        <v>-0.31606528815099999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-0.32</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="5">
+        <v>-5.04</v>
+      </c>
+      <c r="M25" s="5">
+        <v>-2.65</v>
+      </c>
+      <c r="N25" s="6">
+        <v>-1.67</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>-2.41</v>
+      </c>
+      <c r="R25" s="5">
+        <v>-2.5099999999999998</v>
+      </c>
+      <c r="S25" s="6">
+        <v>-2.57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="5">
-        <v>-0.92752680879500005</v>
+        <v>-1.01</v>
       </c>
       <c r="C26" s="5">
-        <v>-1.1194357614699999</v>
+        <v>-1.1399999999999999</v>
       </c>
       <c r="D26" s="6">
-        <v>-1.1806053993100001</v>
+        <v>-1.2</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G26" s="5">
-        <v>-0.28420294037999999</v>
+        <v>-0.3</v>
       </c>
       <c r="H26" s="5">
-        <v>-0.47523417234300003</v>
+        <v>-0.49</v>
       </c>
       <c r="I26" s="6">
-        <v>-0.53623930319500002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="5">
+        <v>-2.93</v>
+      </c>
+      <c r="M26" s="5">
+        <v>-1.51</v>
+      </c>
+      <c r="N26" s="6">
+        <v>-0.86</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>-2.72</v>
+      </c>
+      <c r="R26" s="5">
+        <v>-2.84</v>
+      </c>
+      <c r="S26" s="6">
+        <v>-2.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="5">
-        <v>-2.0982069058800001</v>
+        <v>-2.17</v>
       </c>
       <c r="C27" s="5">
-        <v>-2.2190548435899999</v>
+        <v>-2.23</v>
       </c>
       <c r="D27" s="6">
-        <v>-2.2694102273699999</v>
+        <v>-2.2799999999999998</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G27" s="5">
-        <v>-1.28830698328</v>
+        <v>-1.3</v>
       </c>
       <c r="H27" s="5">
-        <v>-1.4128763496300001</v>
+        <v>-1.42</v>
       </c>
       <c r="I27" s="6">
-        <v>-1.4636778993299999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-1.47</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="5">
+        <v>-2.14</v>
+      </c>
+      <c r="M27" s="5">
+        <v>-1.17</v>
+      </c>
+      <c r="N27" s="6">
+        <v>-0.71</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>-3.87</v>
+      </c>
+      <c r="R27" s="5">
+        <v>-3.93</v>
+      </c>
+      <c r="S27" s="6">
+        <v>-3.98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="5">
-        <v>-2.8672619583399999</v>
+        <v>-2.95</v>
       </c>
       <c r="C28" s="5">
-        <v>-2.7825001470099999</v>
+        <v>-2.8</v>
       </c>
       <c r="D28" s="6">
-        <v>-2.8379532146600002</v>
+        <v>-2.86</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="5">
-        <v>-1.6849458690800001</v>
+        <v>-1.7</v>
       </c>
       <c r="H28" s="5">
-        <v>-1.6003659992099999</v>
+        <v>-1.61</v>
       </c>
       <c r="I28" s="6">
-        <v>-1.65623116083</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-1.67</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="5">
+        <v>-1.65</v>
+      </c>
+      <c r="M28" s="5">
+        <v>-1.26</v>
+      </c>
+      <c r="N28" s="6">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>-4.59</v>
+      </c>
+      <c r="R28" s="5">
+        <v>-4.4400000000000004</v>
+      </c>
+      <c r="S28" s="6">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="5">
-        <v>-3.0021838767400002</v>
+        <v>-3.08</v>
       </c>
       <c r="C29" s="5">
-        <v>-2.9504165036500001</v>
+        <v>-2.96</v>
       </c>
       <c r="D29" s="6">
-        <v>-3.0053687184600002</v>
+        <v>-3.02</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="5">
-        <v>-1.6342493922900001</v>
+        <v>-1.64</v>
       </c>
       <c r="H29" s="5">
-        <v>-1.5881250870700001</v>
+        <v>-1.6</v>
       </c>
       <c r="I29" s="6">
-        <v>-1.6420683148399999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-1.65</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="5">
+        <v>-0.06</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>-4.7699999999999996</v>
+      </c>
+      <c r="R29" s="5">
+        <v>-4.66</v>
+      </c>
+      <c r="S29" s="6">
+        <v>-4.71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="5">
-        <v>0.799796966399</v>
+        <v>0.71</v>
       </c>
       <c r="C30" s="5">
-        <v>0.900224301906</v>
+        <v>0.87</v>
       </c>
       <c r="D30" s="6">
-        <v>0.86861148353899997</v>
+        <v>0.84</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G30" s="5">
-        <v>1.42350844229</v>
+        <v>1.4</v>
       </c>
       <c r="H30" s="5">
-        <v>1.5263307100400001</v>
+        <v>1.5</v>
       </c>
       <c r="I30" s="6">
-        <v>1.49485262758</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.47</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="8">
+        <v>-0.79</v>
+      </c>
+      <c r="M30" s="8">
+        <v>-0.79</v>
+      </c>
+      <c r="N30" s="9">
+        <v>-0.78</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>-1.17</v>
+      </c>
+      <c r="R30" s="5">
+        <v>-1.02</v>
+      </c>
+      <c r="S30" s="6">
+        <v>-1.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="5">
-        <v>0.94700939301300002</v>
+        <v>0.86</v>
       </c>
       <c r="C31" s="5">
-        <v>0.95126668745499998</v>
+        <v>0.93</v>
       </c>
       <c r="D31" s="6">
-        <v>0.91775933079000005</v>
+        <v>0.89</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="5">
-        <v>1.4983949616400001</v>
+        <v>1.48</v>
       </c>
       <c r="H31" s="5">
-        <v>1.5651575102399999</v>
+        <v>1.54</v>
       </c>
       <c r="I31" s="6">
-        <v>1.5319842933400001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.51</v>
+      </c>
+      <c r="K31" s="18"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="P31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="R31" s="5">
+        <v>-0.54</v>
+      </c>
+      <c r="S31" s="6">
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="5">
-        <v>0.26115494572499998</v>
+        <v>0.18</v>
       </c>
       <c r="C32" s="5">
-        <v>9.1602053754500007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D32" s="6">
-        <v>4.2056573775699997E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G32" s="5">
-        <v>0.73136284485199998</v>
+        <v>0.72</v>
       </c>
       <c r="H32" s="5">
-        <v>0.56212222719899996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I32" s="6">
-        <v>0.51277462152200004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+      <c r="K32" s="18"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="P32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>-1.49</v>
+      </c>
+      <c r="R32" s="5">
+        <v>-1.59</v>
+      </c>
+      <c r="S32" s="6">
+        <v>-1.64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="8">
-        <v>-0.70239567723499996</v>
+        <v>-0.78</v>
       </c>
       <c r="C33" s="8">
-        <v>-0.84077621433000005</v>
+        <v>-0.86</v>
       </c>
       <c r="D33" s="9">
-        <v>-0.89850609336999998</v>
+        <v>-0.91</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="8">
-        <v>0.25918632788099999</v>
+        <v>0.25</v>
       </c>
       <c r="H33" s="8">
-        <v>0.19426396413899999</v>
+        <v>0.18</v>
       </c>
       <c r="I33" s="9">
-        <v>0.140159811474</v>
+        <v>0.13</v>
+      </c>
+      <c r="K33" s="18"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="P33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>-2.2599999999999998</v>
+      </c>
+      <c r="R33" s="8">
+        <v>-2.29</v>
+      </c>
+      <c r="S33" s="9">
+        <v>-2.35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A17:I17"/>
+  <mergeCells count="24">
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="K17:S17"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="P19:S19"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="Q20:S20"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:I4"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="A17:I17"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="F4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.02</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5">
+        <v>-1.21</v>
+      </c>
+      <c r="H6" s="5">
+        <v>-0.65</v>
+      </c>
+      <c r="I6" s="6">
+        <v>-0.46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1.82</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.83</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.84</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.34</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.34</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.74</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.74</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.74</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-1.64</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.73</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5">
+        <v>-3.12</v>
+      </c>
+      <c r="H9" s="5">
+        <v>-0.73</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.47</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5">
+        <v>-1.01</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.41</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2.23</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2.69</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="5">
+        <v>-0.22</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.75</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2.14</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2.25</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3.34</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3.68</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3.87</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1.86</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I13" s="6">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2.61</v>
+      </c>
+      <c r="C14" s="8">
+        <v>2.62</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2.62</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="F20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1.18</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1.07</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1.03</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1.07</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="H24" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I24" s="6">
+        <v>-0.13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.81</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="H25" s="5">
+        <v>-0.27</v>
+      </c>
+      <c r="I25" s="6">
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.48</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="H26" s="5">
+        <v>-0.49</v>
+      </c>
+      <c r="I26" s="6">
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="5">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="C27" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="D27" s="6">
+        <v>-0.65</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="5">
+        <v>-1.3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>-1.42</v>
+      </c>
+      <c r="I27" s="6">
+        <v>-1.47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5">
+        <v>-1.27</v>
+      </c>
+      <c r="C28" s="5">
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="D28" s="6">
+        <v>-1.18</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="5">
+        <v>-1.7</v>
+      </c>
+      <c r="H28" s="5">
+        <v>-1.61</v>
+      </c>
+      <c r="I28" s="6">
+        <v>-1.67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="5">
+        <v>-1.45</v>
+      </c>
+      <c r="C29" s="5">
+        <v>-1.33</v>
+      </c>
+      <c r="D29" s="6">
+        <v>-1.39</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="5">
+        <v>-1.64</v>
+      </c>
+      <c r="H29" s="5">
+        <v>-1.6</v>
+      </c>
+      <c r="I29" s="6">
+        <v>-1.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2.15</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D30" s="6">
+        <v>2.27</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="H30" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="I30" s="6">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2.75</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2.78</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2.75</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1.48</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1.54</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1.83</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1.73</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1.68</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.98</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A17:I17"/>
     <mergeCell ref="A19:D19"/>
+    <mergeCell ref="F19:I19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>